<commit_message>
fixes #216, add additional facebook size
</commit_message>
<xml_diff>
--- a/spec/fixtures/io_files/Collective_IO_facebook_li.xlsx
+++ b/spec/fixtures/io_files/Collective_IO_facebook_li.xlsx
@@ -25,25 +25,28 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="175">
   <si>
     <t>Date:</t>
   </si>
@@ -189,6 +192,9 @@
   </si>
   <si>
     <t>Age 18-34 or Age 34-50 or Education; Columbus Zips</t>
+  </si>
+  <si>
+    <t>Facebook – 100x72</t>
   </si>
   <si>
     <t>RON; Columbus Zips</t>
@@ -1401,7 +1407,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1471,15 +1477,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>293760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>498600</xdr:colOff>
+      <xdr:colOff>525240</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1494,8 +1500,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266760" y="174600"/>
-          <a:ext cx="1229760" cy="597600"/>
+          <a:off x="293760" y="165600"/>
+          <a:ext cx="1229400" cy="597240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1510,15 +1516,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>38160</xdr:colOff>
+      <xdr:colOff>64800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1527,8 +1533,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="12600"/>
-          <a:ext cx="12353760" cy="45360"/>
+          <a:off x="189000" y="3600"/>
+          <a:ext cx="12353400" cy="45000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1549,15 +1555,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>38160</xdr:colOff>
+      <xdr:colOff>64800</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1566,8 +1572,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="841320"/>
-          <a:ext cx="12353760" cy="44640"/>
+          <a:off x="189000" y="832320"/>
+          <a:ext cx="12353400" cy="44280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1588,15 +1594,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>102600</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1605,8 +1611,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="4716000"/>
-          <a:ext cx="12391560" cy="141120"/>
+          <a:off x="189000" y="4707000"/>
+          <a:ext cx="12391200" cy="140760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1627,15 +1633,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>66600</xdr:colOff>
+      <xdr:colOff>93240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1644,8 +1650,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="2927160"/>
-          <a:ext cx="12382200" cy="43920"/>
+          <a:off x="189000" y="2918160"/>
+          <a:ext cx="12381840" cy="43560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1671,15 +1677,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>219240</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>283680</xdr:colOff>
+      <xdr:colOff>310320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>201240</xdr:rowOff>
+      <xdr:rowOff>200880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1694,8 +1700,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="219240" y="3240"/>
-          <a:ext cx="1595880" cy="721800"/>
+          <a:off x="246240" y="3240"/>
+          <a:ext cx="1595520" cy="721440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1715,15 +1721,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>293760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>357840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>249120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1738,8 +1744,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266760" y="60480"/>
-          <a:ext cx="1595880" cy="721800"/>
+          <a:off x="293760" y="51480"/>
+          <a:ext cx="1595520" cy="721440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1759,15 +1765,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>293760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>357840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>201240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1782,8 +1788,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266760" y="12600"/>
-          <a:ext cx="1595880" cy="721800"/>
+          <a:off x="293760" y="3600"/>
+          <a:ext cx="1595520" cy="721440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1805,7 +1811,7 @@
   </sheetPr>
   <dimension ref="A1:AI172"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A20" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A14" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A31" activeCellId="0" pane="topLeft" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -2615,10 +2621,10 @@
         <v>41515</v>
       </c>
       <c r="C30" s="56" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D30" s="61" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E30" s="61"/>
       <c r="F30" s="58" t="n">
@@ -2630,7 +2636,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="31" s="5">
       <c r="A31" s="62" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" s="62"/>
       <c r="C31" s="62"/>
@@ -2690,10 +2696,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="21.75" outlineLevel="0" r="33" s="5">
       <c r="A33" s="68" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C33" s="69"/>
       <c r="D33" s="69"/>
@@ -2798,11 +2804,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="38">
       <c r="A38" s="70" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B38" s="71"/>
       <c r="C38" s="72" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D38" s="71"/>
       <c r="E38" s="71"/>
@@ -2814,7 +2820,7 @@
       <c r="A39" s="70"/>
       <c r="B39" s="71"/>
       <c r="C39" s="72" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D39" s="71"/>
       <c r="E39" s="71"/>
@@ -2834,11 +2840,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="72" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B41" s="71"/>
       <c r="C41" s="72" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D41" s="71"/>
       <c r="E41" s="71"/>
@@ -2858,11 +2864,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="72" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B43" s="71"/>
       <c r="C43" s="73" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D43" s="73"/>
       <c r="E43" s="73"/>
@@ -2892,11 +2898,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="A46" s="72" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B46" s="72"/>
       <c r="C46" s="75" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D46" s="75"/>
       <c r="E46" s="75"/>
@@ -2936,11 +2942,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="50">
       <c r="A50" s="72" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B50" s="72"/>
       <c r="C50" s="75" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D50" s="75"/>
       <c r="E50" s="75"/>
@@ -2980,11 +2986,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="A54" s="72" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B54" s="72"/>
       <c r="C54" s="75" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D54" s="75"/>
       <c r="E54" s="75"/>
@@ -3024,7 +3030,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="58">
       <c r="A58" s="72" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58" s="72"/>
       <c r="C58" s="72"/>
@@ -3076,17 +3082,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="63">
       <c r="A63" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H63" s="4"/>
     </row>
@@ -4278,7 +4284,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="172">
       <c r="I172" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4349,25 +4355,25 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="78" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
       <c r="D3" s="78"/>
       <c r="E3" s="78" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F3" s="78"/>
       <c r="G3" s="78" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I3" s="78" t="s">
         <v>36</v>
@@ -4376,13 +4382,13 @@
         <v>37</v>
       </c>
       <c r="K3" s="78" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L3" s="78" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4">
@@ -4391,26 +4397,26 @@
         <v>0</v>
       </c>
       <c r="B4" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D4" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E4" s="81" t="n">
         <v>78002775</v>
       </c>
       <c r="F4" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G4" s="79" t="str">
         <f aca="false">'Insertion Order'!D29</f>
         <v>Age 18-34 or Age 34-50 or Education; Columbus Zips</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I4" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4429,7 +4435,7 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=78002775;sz=300x250</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
@@ -4438,24 +4444,24 @@
         <v>0</v>
       </c>
       <c r="B5" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C5" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D5" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G5" s="79" t="str">
         <f aca="false">'Insertion Order'!D30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I5" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4480,24 +4486,24 @@
         <v>0</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E6" s="79"/>
       <c r="F6" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G6" s="79" t="str">
         <f aca="false">'Insertion Order'!D30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H6" s="79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I6" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4516,7 +4522,7 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=160x600</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
@@ -4525,24 +4531,24 @@
         <v>0</v>
       </c>
       <c r="B7" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G7" s="79" t="str">
         <f aca="false">'Insertion Order'!$D$30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H7" s="79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I7" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4561,7 +4567,7 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=300x250</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
@@ -4570,24 +4576,24 @@
         <v>0</v>
       </c>
       <c r="B8" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D8" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E8" s="83"/>
       <c r="F8" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G8" s="79" t="str">
         <f aca="false">'Insertion Order'!$D$30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H8" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I8" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4606,7 +4612,7 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=728x90</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
@@ -4615,24 +4621,24 @@
         <v>0</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E9" s="79"/>
       <c r="F9" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G9" s="79" t="str">
         <f aca="false">'Insertion Order'!$D$30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H9" s="79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I9" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4653,22 +4659,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="R10" s="78" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="R11" s="79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="R12" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="R13" s="79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4727,7 +4733,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
       <c r="C3" s="84"/>
       <c r="D3" s="85" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E3" s="86"/>
       <c r="F3" s="86"/>
@@ -4736,55 +4742,55 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.1" outlineLevel="0" r="4"/>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="90">
       <c r="A5" s="87" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G5" s="87" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H5" s="88" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J5" s="87" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K5" s="87" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L5" s="87" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M5" s="88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N5" s="88" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O5" s="88" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P5" s="88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q5" s="87" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R5" s="89"/>
     </row>
@@ -4810,260 +4816,260 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="101">
       <c r="A7" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H7" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J7" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K7" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L7" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M7" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N7" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O7" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P7" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="99"/>
       <c r="R7" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="101">
       <c r="A8" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E8" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F8" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G8" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H8" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J8" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K8" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L8" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M8" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N8" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O8" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P8" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q8" s="99"/>
       <c r="R8" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="101">
       <c r="A9" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B9" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C9" s="95" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E9" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F9" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G9" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H9" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I9" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J9" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K9" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L9" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M9" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N9" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O9" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P9" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q9" s="99"/>
       <c r="R9" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="101">
       <c r="A10" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" s="95" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D10" s="94" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E10" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F10" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G10" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H10" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I10" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J10" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K10" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L10" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M10" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N10" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O10" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P10" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q10" s="99"/>
       <c r="R10" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="101">
       <c r="A11" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B11" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C11" s="95" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E11" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F11" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G11" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H11" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I11" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J11" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K11" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L11" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M11" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N11" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O11" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P11" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q11" s="99"/>
       <c r="R11" s="100"/>
@@ -5140,88 +5146,88 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
       <c r="C3" s="84"/>
       <c r="D3" s="85" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="4"/>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.75" outlineLevel="0" r="5" s="90">
       <c r="A5" s="87" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G5" s="87" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H5" s="87" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J5" s="88" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K5" s="87" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L5" s="87" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M5" s="87" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N5" s="88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O5" s="88" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P5" s="88" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q5" s="88" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="R5" s="88" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="S5" s="88" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="T5" s="88" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="U5" s="88" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="V5" s="87" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="W5" s="88" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X5" s="88" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Y5" s="88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Z5" s="87" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA5" s="89"/>
     </row>
@@ -5256,395 +5262,395 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="101">
       <c r="A7" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H7" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J7" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K7" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L7" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M7" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N7" s="96" t="n">
         <v>24</v>
       </c>
       <c r="O7" s="97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P7" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q7" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R7" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S7" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T7" s="96" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="U7" s="96" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="V7" s="95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W7" s="97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X7" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y7" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z7" s="99"/>
       <c r="AA7" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="101">
       <c r="A8" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E8" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F8" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G8" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H8" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J8" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K8" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L8" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M8" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N8" s="96" t="n">
         <v>24</v>
       </c>
       <c r="O8" s="97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P8" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q8" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R8" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S8" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T8" s="96" t="s">
+        <v>146</v>
+      </c>
+      <c r="U8" s="96" t="s">
+        <v>147</v>
+      </c>
+      <c r="V8" s="95" t="s">
+        <v>144</v>
+      </c>
+      <c r="W8" s="97" t="s">
         <v>145</v>
       </c>
-      <c r="U8" s="96" t="s">
-        <v>146</v>
-      </c>
-      <c r="V8" s="95" t="s">
-        <v>143</v>
-      </c>
-      <c r="W8" s="97" t="s">
-        <v>144</v>
-      </c>
       <c r="X8" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y8" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z8" s="99"/>
       <c r="AA8" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="101">
       <c r="A9" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B9" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C9" s="95" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E9" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F9" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G9" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H9" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I9" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J9" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K9" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L9" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M9" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N9" s="96" t="n">
         <v>24</v>
       </c>
       <c r="O9" s="97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P9" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q9" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R9" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S9" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T9" s="96" t="s">
+        <v>148</v>
+      </c>
+      <c r="U9" s="96" t="s">
         <v>147</v>
       </c>
-      <c r="U9" s="96" t="s">
-        <v>146</v>
-      </c>
       <c r="V9" s="95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W9" s="97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X9" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y9" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z9" s="99"/>
       <c r="AA9" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="101">
       <c r="A10" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" s="95" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D10" s="94" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E10" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F10" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G10" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H10" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I10" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J10" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K10" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L10" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M10" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N10" s="96" t="n">
         <v>24</v>
       </c>
       <c r="O10" s="97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P10" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q10" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R10" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S10" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T10" s="96" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="U10" s="96" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="V10" s="95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W10" s="97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X10" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y10" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z10" s="99"/>
       <c r="AA10" s="100"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11">
       <c r="A11" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B11" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C11" s="95" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E11" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F11" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G11" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H11" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I11" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J11" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K11" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L11" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M11" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N11" s="107" t="n">
         <v>24</v>
       </c>
       <c r="O11" s="108" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P11" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q11" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R11" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S11" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T11" s="96" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="U11" s="96" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="V11" s="95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W11" s="97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X11" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y11" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z11" s="99"/>
       <c r="AA11" s="100"/>
@@ -5722,7 +5728,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
       <c r="C3" s="109" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D3" s="85"/>
       <c r="E3" s="85"/>
@@ -5732,49 +5738,49 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.95" outlineLevel="0" r="4"/>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="90">
       <c r="A5" s="87" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B5" s="111" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G5" s="87" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H5" s="87" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J5" s="88" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K5" s="88" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L5" s="88" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M5" s="88" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N5" s="88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O5" s="87" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P5" s="89"/>
     </row>
@@ -5798,97 +5804,97 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="101">
       <c r="A7" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="112" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H7" s="94" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I7" s="94" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J7" s="96" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K7" s="96" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L7" s="97" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M7" s="96" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N7" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O7" s="113" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P7" s="100"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="8">
       <c r="A8" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="112" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="114" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="94" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="114" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" s="114" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" s="94" t="s">
+        <v>167</v>
+      </c>
+      <c r="J8" s="96" t="s">
+        <v>168</v>
+      </c>
+      <c r="K8" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="M8" s="96" t="s">
+        <v>170</v>
+      </c>
+      <c r="N8" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="O8" s="113" t="s">
         <v>171</v>
-      </c>
-      <c r="C8" s="95" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" s="94" t="s">
-        <v>173</v>
-      </c>
-      <c r="E8" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F8" s="94" t="s">
-        <v>163</v>
-      </c>
-      <c r="G8" s="114" t="s">
-        <v>164</v>
-      </c>
-      <c r="H8" s="114" t="s">
-        <v>165</v>
-      </c>
-      <c r="I8" s="94" t="s">
-        <v>166</v>
-      </c>
-      <c r="J8" s="96" t="s">
-        <v>167</v>
-      </c>
-      <c r="K8" s="96" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="97" t="s">
-        <v>168</v>
-      </c>
-      <c r="M8" s="96" t="s">
-        <v>169</v>
-      </c>
-      <c r="N8" s="106" t="s">
-        <v>114</v>
-      </c>
-      <c r="O8" s="113" t="s">
-        <v>170</v>
       </c>
       <c r="P8" s="100"/>
     </row>

</xml_diff>